<commit_message>
changes to scripts inventory (unclear what) but possibly just because it was opened
</commit_message>
<xml_diff>
--- a/documents/scripts_inventory.xlsx
+++ b/documents/scripts_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8693BF0-78D9-8C4A-AEF2-AD1BC30F28EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660AF6E4-18A0-944B-B8BF-9CF933B82B07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{9581F75B-0F49-B149-888E-54709FBADFF3}"/>
   </bookViews>
@@ -762,7 +762,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
edits made when trying to figure out what the latest version of text c&ped was before changed to 1s & 0s [which i believe is codesalafsky --> should come after AS9_codingdata]
so added some info to pre-existing rows and also added some new data points/csv file names that have been made since
</commit_message>
<xml_diff>
--- a/documents/scripts_inventory.xlsx
+++ b/documents/scripts_inventory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/usr/local/bin/store/partner_rff/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660AF6E4-18A0-944B-B8BF-9CF933B82B07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFA21F6-126E-6248-8C84-9A664636C50B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14700" xr2:uid="{9581F75B-0F49-B149-888E-54709FBADFF3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="135">
   <si>
     <t>name of script</t>
   </si>
@@ -397,6 +397,39 @@
   </si>
   <si>
     <t>Need to add what function produced them to title of csv??</t>
+  </si>
+  <si>
+    <t>tableofpartnersandactions</t>
+  </si>
+  <si>
+    <t>tableofPandA</t>
+  </si>
+  <si>
+    <t>started as copy of tablesofpartnersandactions.csv so that an extra column could be added and org types could be assigned to each partner row</t>
+  </si>
+  <si>
+    <t>tableofpartnersandactions.csv (but not created in a script)</t>
+  </si>
+  <si>
+    <t>finalSdataset_8_29.csv</t>
+  </si>
+  <si>
+    <t>Includes all actions org types and species in finished product</t>
+  </si>
+  <si>
+    <t>** I think this is the latest version of salafsky coding actions (came after AS_9_coding) where actions are 1s and 0s</t>
+  </si>
+  <si>
+    <t>** latest version of salafsky actions categorization before text was changed to 1s and 0s</t>
+  </si>
+  <si>
+    <t>Partnerships_draft_code</t>
+  </si>
+  <si>
+    <t>this csv file</t>
+  </si>
+  <si>
+    <t>combined with correct names of partners and collabs, fixed spelling issues, and assigned correct orgtypes</t>
   </si>
 </sst>
 </file>
@@ -758,11 +791,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53DF7BFE-6949-4246-AC39-BB06848EDA9D}">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,6 +1130,12 @@
       <c r="E14" t="s">
         <v>9</v>
       </c>
+      <c r="I14" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
@@ -1570,6 +1609,9 @@
       <c r="J36" t="s">
         <v>118</v>
       </c>
+      <c r="L36" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
@@ -1589,6 +1631,66 @@
       </c>
       <c r="I37" t="s">
         <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" t="s">
+        <v>126</v>
+      </c>
+      <c r="G38" t="s">
+        <v>9</v>
+      </c>
+      <c r="H38" t="s">
+        <v>120</v>
+      </c>
+      <c r="I38" t="s">
+        <v>127</v>
+      </c>
+      <c r="J38" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" t="s">
+        <v>129</v>
+      </c>
+      <c r="I39" t="s">
+        <v>104</v>
+      </c>
+      <c r="J39" t="s">
+        <v>132</v>
+      </c>
+      <c r="K39" t="s">
+        <v>133</v>
+      </c>
+      <c r="L39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>77</v>
+      </c>
+      <c r="L40" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>